<commit_message>
data updated at 13 Dec 9AM
</commit_message>
<xml_diff>
--- a/Daily Orders/December-2020-RetailerWiseOrder.xlsx
+++ b/Daily Orders/December-2020-RetailerWiseOrder.xlsx
@@ -336,11 +336,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -360,7 +360,84 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -368,6 +445,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -389,32 +473,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -428,68 +488,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -497,7 +497,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -536,13 +536,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -554,127 +560,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -692,7 +578,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -704,19 +686,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -730,26 +730,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -769,37 +769,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -822,8 +802,28 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -832,10 +832,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -850,130 +850,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -993,7 +993,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1335,11 +1335,11 @@
   <dimension ref="A1:AJ92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="M48" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N44" sqref="N44"/>
+      <selection pane="bottomRight" activeCell="R69" sqref="R69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1468,11 +1468,11 @@
       </c>
       <c r="D2" s="7">
         <f>E2/1.04</f>
-        <v>482500</v>
+        <v>488500</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(F2:AJ2)</f>
-        <v>501800</v>
+        <v>508040</v>
       </c>
       <c r="F2" s="2">
         <f>SUM(F3:F92)</f>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="R2" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6240</v>
       </c>
       <c r="S2" s="2">
         <f t="shared" si="1"/>
@@ -1843,7 +1843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:18">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1855,11 +1855,11 @@
       </c>
       <c r="D13" s="9">
         <f t="shared" si="2"/>
-        <v>7000</v>
+        <v>10000</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="3"/>
-        <v>7280</v>
+        <v>10400</v>
       </c>
       <c r="I13" s="3">
         <v>2080</v>
@@ -1868,6 +1868,9 @@
         <v>2080</v>
       </c>
       <c r="M13" s="3">
+        <v>3120</v>
+      </c>
+      <c r="R13" s="3">
         <v>3120</v>
       </c>
     </row>
@@ -3155,7 +3158,7 @@
         <v>1560</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:18">
       <c r="A68" s="3">
         <v>66</v>
       </c>
@@ -3167,16 +3170,19 @@
       </c>
       <c r="D68" s="9">
         <f t="shared" si="6"/>
-        <v>5000</v>
+        <v>8000</v>
       </c>
       <c r="E68" s="2">
         <f t="shared" si="7"/>
-        <v>5200</v>
+        <v>8320</v>
       </c>
       <c r="N68" s="3">
         <v>2080</v>
       </c>
       <c r="O68" s="3">
+        <v>3120</v>
+      </c>
+      <c r="R68" s="3">
         <v>3120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data updated till 14-dec-2020 9AM
</commit_message>
<xml_diff>
--- a/Daily Orders/December-2020-RetailerWiseOrder.xlsx
+++ b/Daily Orders/December-2020-RetailerWiseOrder.xlsx
@@ -347,8 +347,8 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="[$-409]d\-mmm;@"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -368,30 +368,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -412,8 +391,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -435,15 +422,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -457,10 +443,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -472,25 +458,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -507,6 +476,37 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -551,19 +551,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -575,7 +629,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -593,31 +689,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -629,67 +713,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -705,36 +735,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -742,45 +742,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -802,8 +763,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -819,6 +780,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -842,12 +827,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -865,130 +865,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1354,11 +1354,11 @@
   <dimension ref="A1:AK92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="L36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L42" sqref="L42"/>
+      <selection pane="bottomRight" activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1490,11 +1490,11 @@
       </c>
       <c r="E2" s="7">
         <f>F2/1.04</f>
-        <v>518500</v>
+        <v>527500</v>
       </c>
       <c r="F2" s="8">
         <f>SUM(G2:AK2)</f>
-        <v>539240</v>
+        <v>548600</v>
       </c>
       <c r="G2" s="2">
         <f>SUM(G3:G92)</f>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="T2" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9360</v>
       </c>
       <c r="U2" s="2">
         <f t="shared" si="1"/>
@@ -1805,7 +1805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:20">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1817,11 +1817,11 @@
       </c>
       <c r="E10" s="9">
         <f t="shared" si="2"/>
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="3"/>
-        <v>6240</v>
+        <v>9360</v>
       </c>
       <c r="I10" s="3">
         <v>1040</v>
@@ -1830,6 +1830,9 @@
         <v>2080</v>
       </c>
       <c r="M10" s="3">
+        <v>3120</v>
+      </c>
+      <c r="T10" s="3">
         <v>3120</v>
       </c>
     </row>
@@ -1896,7 +1899,7 @@
         <v>3120</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:20">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1908,13 +1911,16 @@
       </c>
       <c r="E14" s="9">
         <f t="shared" si="2"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="3"/>
-        <v>2080</v>
+        <v>4160</v>
       </c>
       <c r="J14" s="3">
+        <v>2080</v>
+      </c>
+      <c r="T14" s="3">
         <v>2080</v>
       </c>
     </row>
@@ -2403,7 +2409,7 @@
         <v>3120</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:20">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -2415,11 +2421,14 @@
       </c>
       <c r="E35" s="9">
         <f t="shared" ref="E35:E66" si="4">F35/1.04</f>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="F35" s="2">
         <f t="shared" ref="F35:F66" si="5">SUM(G35:AK35)</f>
-        <v>0</v>
+        <v>2080</v>
+      </c>
+      <c r="T35" s="10">
+        <v>2080</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -3547,7 +3556,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:20">
       <c r="A81" s="3">
         <v>79</v>
       </c>
@@ -3562,11 +3571,14 @@
       </c>
       <c r="E81" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="F81" s="2">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2080</v>
+      </c>
+      <c r="T81" s="3">
+        <v>2080</v>
       </c>
     </row>
     <row r="82" spans="1:18">

</xml_diff>